<commit_message>
+ completed the report
</commit_message>
<xml_diff>
--- a/docs/supplier/ProjectSummary.xlsx
+++ b/docs/supplier/ProjectSummary.xlsx
@@ -8,15 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="46">
   <si>
     <t>Iteration Number</t>
   </si>
@@ -112,6 +110,48 @@
   </si>
   <si>
     <t>Save user information</t>
+  </si>
+  <si>
+    <t>Track patients information</t>
+  </si>
+  <si>
+    <t>Add validation of user input</t>
+  </si>
+  <si>
+    <t>Nurse checks in/out patients</t>
+  </si>
+  <si>
+    <t>Patients change bed</t>
+  </si>
+  <si>
+    <t>A doctor or a head nurse can enter nurses' information</t>
+  </si>
+  <si>
+    <t>Implement permissions</t>
+  </si>
+  <si>
+    <t>Nurses can view information of the patients that they are in charge of</t>
+  </si>
+  <si>
+    <t>A secretary can enter patients' information when they arrive</t>
+  </si>
+  <si>
+    <t>An administrator assigns a nurse to a ward</t>
+  </si>
+  <si>
+    <t>An administrator or a nurse assigns a patient to a room</t>
+  </si>
+  <si>
+    <t>A doctor or a nurse can search for a patient</t>
+  </si>
+  <si>
+    <t>Search for patients</t>
+  </si>
+  <si>
+    <t>View nurses in wards</t>
+  </si>
+  <si>
+    <t>Show ward names instead of numbers in the table</t>
   </si>
 </sst>
 </file>
@@ -330,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -374,16 +414,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -678,17 +717,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:G18"/>
+  <dimension ref="B2:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="24" customWidth="1"/>
-    <col min="3" max="3" width="4.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="49.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="38" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="1"/>
@@ -700,17 +737,17 @@
       <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="29" t="s">
+      <c r="D2" s="31"/>
+      <c r="E2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="28" t="s">
         <v>4</v>
       </c>
     </row>
@@ -753,16 +790,16 @@
       <c r="C5" s="4">
         <v>1.2</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="31" t="s">
+      <c r="F5" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="30" t="s">
         <v>24</v>
       </c>
     </row>
@@ -957,33 +994,259 @@
       </c>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="27"/>
-      <c r="C17" s="7">
+      <c r="B17" s="26"/>
+      <c r="C17" s="4">
         <f t="shared" si="0"/>
         <v>2.8000000000000007</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="21"/>
-      <c r="F17" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" s="20" t="s">
+      <c r="E17" s="15"/>
+      <c r="F17" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="14" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="32">
+      <c r="B18" s="25">
         <v>3</v>
       </c>
       <c r="C18" s="3">
         <v>3.1</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="13"/>
+      <c r="D18" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="B19" s="26"/>
+      <c r="C19" s="4">
+        <f>C18+0.1</f>
+        <v>3.2</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" s="26"/>
+      <c r="C20" s="3">
+        <f t="shared" ref="C20:C28" si="1">C19+0.1</f>
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="B21" s="26"/>
+      <c r="C21" s="4">
+        <f t="shared" si="1"/>
+        <v>3.4000000000000004</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="B22" s="26"/>
+      <c r="C22" s="3">
+        <f t="shared" si="1"/>
+        <v>3.5000000000000004</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="B23" s="26"/>
+      <c r="C23" s="4">
+        <f t="shared" si="1"/>
+        <v>3.6000000000000005</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="15"/>
+      <c r="F23" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="B24" s="26"/>
+      <c r="C24" s="3">
+        <f t="shared" si="1"/>
+        <v>3.7000000000000006</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="B25" s="26"/>
+      <c r="C25" s="4">
+        <f t="shared" si="1"/>
+        <v>3.8000000000000007</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="B26" s="26"/>
+      <c r="C26" s="3">
+        <f t="shared" si="1"/>
+        <v>3.9000000000000008</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="B27" s="26"/>
+      <c r="C27" s="4">
+        <v>3.1</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="B28" s="26"/>
+      <c r="C28" s="2">
+        <v>3.11</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7">
+      <c r="B29" s="26"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="F29" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="G29" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7">
+      <c r="B30" s="27"/>
+      <c r="C30" s="7">
+        <v>3.12</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="F30" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="G30" s="20" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -992,28 +1255,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>